<commit_message>
Laboratory 01: Removing Trend and Seasonality in Time Series
</commit_message>
<xml_diff>
--- a/labs/01_trend_and_seasonality/excel/removing_trend_and_seasonality.xlsx
+++ b/labs/01_trend_and_seasonality/excel/removing_trend_and_seasonality.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielfaltynowski/Documents/Repositories/time-series-labs/labs/01_trend_and_seasonality/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielfaltynowski/Documents/Repositories/time-series-labs/labs/01_trend_and_seasonality/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E45E28F-D2DC-DE4E-886B-F1FA2D91934F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64579B7-5CDC-734D-AF60-9DDED134825A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16020" xr2:uid="{89C6EF17-6D7C-1E4E-801A-59B52683BE08}"/>
   </bookViews>
@@ -623,6 +623,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>GVA</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -866,6 +869,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>GVA (no trend)</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1109,6 +1115,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>GVA (no trend &amp; no seasonality)</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1499,6 +1508,34 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2521,8 +2558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7642CC08-B680-3746-A0EB-52269A8A055A}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>